<commit_message>
Note toegevoegd dat we niet aan de product vision hadden gedacht
</commit_message>
<xml_diff>
--- a/SE Deliverables/Week 2/Sprint reflection 1.xlsx
+++ b/SE Deliverables/Week 2/Sprint reflection 1.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="43">
   <si>
     <t>User Story</t>
   </si>
@@ -146,6 +146,9 @@
   </si>
   <si>
     <t>Noone</t>
+  </si>
+  <si>
+    <t>We did not anticipate having to write a report</t>
   </si>
 </sst>
 </file>
@@ -334,16 +337,16 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1680,10 +1683,10 @@
   <dimension ref="A1:IX21"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozenSplit"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="C13" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="D16" sqref="D16"/>
+      <selection pane="bottomRight" activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1700,14 +1703,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="16.2" x14ac:dyDescent="0.25">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
-      <c r="F1" s="10"/>
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="12"/>
+      <c r="F1" s="12"/>
     </row>
     <row r="2" spans="1:9" ht="39.6" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
@@ -1964,8 +1967,8 @@
       </c>
     </row>
     <row r="12" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="12"/>
-      <c r="B12" s="11"/>
+      <c r="A12" s="10"/>
+      <c r="B12" s="9"/>
       <c r="C12" s="4"/>
       <c r="D12" s="4"/>
       <c r="E12" s="4"/>
@@ -2006,7 +2009,9 @@
       <c r="H14" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="I14" s="4"/>
+      <c r="I14" s="4" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="15" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="3"/>

</xml_diff>